<commit_message>
Changed LED part # for fixed 5V 630nm design.
</commit_message>
<xml_diff>
--- a/fixed/5V_regulator/630nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_630nm_16mA.xlsx
+++ b/fixed/5V_regulator/630nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_630nm_16mA.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">0603</t>
   </si>
   <si>
-    <t xml:space="preserve"> C375444</t>
+    <t xml:space="preserve">C5349935</t>
   </si>
   <si>
     <t xml:space="preserve">4-Pin Connector, JST SM04B-SRSS-TB</t>
@@ -434,7 +434,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Change part # for 630nm led design.
</commit_message>
<xml_diff>
--- a/fixed/5V_regulator/630nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_630nm_16mA.xlsx
+++ b/fixed/5V_regulator/630nm_16mA/production/ver_0p1_rev_2/BOM_JLCPCB_630nm_16mA.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">0603</t>
   </si>
   <si>
-    <t xml:space="preserve">C5349935</t>
+    <t xml:space="preserve">C193902</t>
   </si>
   <si>
     <t xml:space="preserve">4-Pin Connector, JST SM04B-SRSS-TB</t>
@@ -434,7 +434,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>